<commit_message>
Add optional output log files for each species model.  Recompile installer.  Add spreadsheet to tests.
</commit_message>
<xml_diff>
--- a/trunk/tests/bird_model_test_transform.xlsx
+++ b/trunk/tests/bird_model_test_transform.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-540" yWindow="375" windowWidth="17235" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="1035" yWindow="120" windowWidth="17235" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="PIWA" sheetId="1" r:id="rId1"/>
-    <sheet name="YBFL" sheetId="4" r:id="rId2"/>
-    <sheet name="OVEN" sheetId="5" r:id="rId3"/>
+    <sheet name="BLBW" sheetId="6" r:id="rId1"/>
+    <sheet name="CONW" sheetId="7" r:id="rId2"/>
+    <sheet name="GWWA" sheetId="8" r:id="rId3"/>
+    <sheet name="PIWA" sheetId="1" r:id="rId4"/>
+    <sheet name="REVI" sheetId="9" r:id="rId5"/>
+    <sheet name="YBFL" sheetId="4" r:id="rId6"/>
+    <sheet name="OVEN" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="56">
   <si>
     <t>int</t>
   </si>
@@ -115,6 +119,75 @@
   </si>
   <si>
     <t>12.95 in output</t>
+  </si>
+  <si>
+    <t>Open1000</t>
+  </si>
+  <si>
+    <t>BLBW</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>CONW</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t>logopen200</t>
+  </si>
+  <si>
+    <t>logreg1000</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>loglc200</t>
+  </si>
+  <si>
+    <t>loglf1000</t>
+  </si>
+  <si>
+    <t>loglf500</t>
+  </si>
+  <si>
+    <t>REVI</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Under ideal conditions for other parameters, avg spring temp must be &lt;= 7.6 for abundance to be &gt;= 0.01</t>
+  </si>
+  <si>
+    <t>Under realistic but favorable conditions, avg spring temp must be &lt;= 5 for abundnace to be &gt;= 0.01</t>
+  </si>
+  <si>
+    <t>Under realistic unfavorable conditinos, avg spring temp must be &lt;= -15.4 for adundance to be &gt;= 0.01</t>
+  </si>
+  <si>
+    <t>Under favorable conditions for other parameters, biomass must be &lt;= 15800 for abundance to be &gt;= 0.01</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Test5</t>
+  </si>
+  <si>
+    <t>Under the best conditions in the Chip Year 0 map, temp must be &lt;= 4.7 for abundance to be &gt;= 0.01</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>GWWA</t>
   </si>
 </sst>
 </file>
@@ -617,7 +690,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -651,9 +724,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -664,6 +734,23 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -717,6 +804,317 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>REVI</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>100% Lowland Conifer</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>REVI!$B$17:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>REVI!$F$17:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.3012768828703487</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5850529724651405</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1353397254784445</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.201614580814022</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.266028270560252</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.259499965384421</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>No LowlandForest</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>REVI!$B$23:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>REVI!$F$23:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.6180191965875594</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2008288129896521</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.331711997100602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.52447343093214</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.772914472960167</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.997476510841892</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="108016768"/>
+        <c:axId val="108018688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="108016768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Biomass (g/m2)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="108018688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="108018688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Abundance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="108016768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15063779527559057"/>
+          <c:y val="0.13850503062117236"/>
+          <c:w val="0.33547331583552054"/>
+          <c:h val="0.16743438320209975"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1006,6 +1404,1063 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="6"/>
+    <col min="3" max="4" width="14.7109375" style="6" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="6"/>
+    <col min="7" max="7" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="16">
+        <v>-2.2350940000000001</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0.40635490000000002</v>
+      </c>
+      <c r="D3" s="16">
+        <v>-3.2001399999999999E-2</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6">
+        <v>100</v>
+      </c>
+      <c r="D6" s="6">
+        <v>100</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6">
+        <f>LOG(C5+1)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <f>LOG(D5+1)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6">
+        <f>LOG(C6+1)</f>
+        <v>2.0043213737826426</v>
+      </c>
+      <c r="D8" s="6">
+        <f>LOG(D6+1)</f>
+        <v>2.0043213737826426</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="20"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="17" t="str">
+        <f>C2</f>
+        <v>LogUC200</v>
+      </c>
+      <c r="C12" s="17" t="str">
+        <f>D2</f>
+        <v>Open1000</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>2</v>
+      </c>
+      <c r="C13" s="6">
+        <v>100</v>
+      </c>
+      <c r="F13" s="6">
+        <f>EXP(B$3+B13*C$3+C13*D$3)</f>
+        <v>9.827956995942539E-3</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6">
+        <v>100</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" ref="F14:F17" si="0">EXP(B$3+B14*C$3+C14*D$3)</f>
+        <v>4.3602146115501294E-3</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="0"/>
+        <v>0.24113840879303725</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="0"/>
+        <v>0.10698207306558467</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="21">
+        <v>0</v>
+      </c>
+      <c r="C17" s="21">
+        <v>7.46</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="6">
+        <f t="shared" si="0"/>
+        <v>8.4261986742040565E-2</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="6">
+        <f>MIN(F13:F16)</f>
+        <v>4.3602146115501294E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="6">
+        <f>MAX(F13:F16)</f>
+        <v>0.24113840879303725</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="I11:K11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="6"/>
+    <col min="3" max="4" width="14.7109375" style="6" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="6"/>
+    <col min="7" max="7" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.70589000000000002</v>
+      </c>
+      <c r="C3" s="16">
+        <v>1.2553099999999999</v>
+      </c>
+      <c r="D3" s="16">
+        <v>-1.9454199999999999</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>34</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6">
+        <v>100</v>
+      </c>
+      <c r="D6" s="6">
+        <v>130</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6">
+        <f>LOG(C5+1)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <f>LOG(D5+1)</f>
+        <v>1.5440680443502757</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6">
+        <f>LOG(C6+1)</f>
+        <v>2.0043213737826426</v>
+      </c>
+      <c r="D8" s="6">
+        <f>LOG(D6+1)</f>
+        <v>2.1172712956557644</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="20"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="17" t="str">
+        <f>C2</f>
+        <v>LogUC200</v>
+      </c>
+      <c r="C12" s="17" t="str">
+        <f>D2</f>
+        <v>LogPrevPrecip</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <f>C8</f>
+        <v>2.0043213737826426</v>
+      </c>
+      <c r="C13" s="6">
+        <f>D8</f>
+        <v>2.1172712956557644</v>
+      </c>
+      <c r="F13" s="6">
+        <f>EXP(B$3+B13*C$3+C13*D$3)</f>
+        <v>0.40777192824677433</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <f>C7</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="6">
+        <f>D8</f>
+        <v>2.1172712956557644</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" ref="F14:F17" si="0">EXP(B$3+B14*C$3+C14*D$3)</f>
+        <v>3.2939197269821127E-2</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <f>C8</f>
+        <v>2.0043213737826426</v>
+      </c>
+      <c r="C15" s="6">
+        <f>D7</f>
+        <v>1.5440680443502757</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2436788587791148</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <f>C7</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="6">
+        <f>D7</f>
+        <v>1.5440680443502757</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="0"/>
+        <v>0.1004624900143683</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="21">
+        <v>0</v>
+      </c>
+      <c r="C17" s="21">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2580376055535952E-7</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="6">
+        <f>MIN(F13:F16)</f>
+        <v>3.2939197269821127E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="6">
+        <f>MAX(F13:F16)</f>
+        <v>1.2436788587791148</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="I11:K11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="9.140625" style="6"/>
+    <col min="7" max="7" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="27">
+        <v>-6.51</v>
+      </c>
+      <c r="C3" s="27">
+        <v>-4.1E-5</v>
+      </c>
+      <c r="D3" s="27">
+        <v>0.93</v>
+      </c>
+      <c r="E3" s="27">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="F3" s="27">
+        <v>-0.20399999999999999</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="F5" s="6">
+        <v>4.0487500000000001</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D6" s="6">
+        <v>78.849999999999994</v>
+      </c>
+      <c r="E6" s="6">
+        <v>99.28</v>
+      </c>
+      <c r="F6" s="6">
+        <v>10.5688</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6">
+        <f>LOG(D5+1)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <f>LOG(E5+1)</f>
+        <v>0.11727129565576427</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="6">
+        <f>LOG(D6+1)</f>
+        <v>1.9022749204745018</v>
+      </c>
+      <c r="E8" s="6">
+        <f>LOG(E6+1)</f>
+        <v>2.0012143252861789</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="26"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="26"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="str">
+        <f>C2</f>
+        <v>biomass</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>D2</f>
+        <v>logopen200</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>E2</f>
+        <v>logreg1000</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f>F2</f>
+        <v>temp</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2</v>
+      </c>
+      <c r="E13" s="6">
+        <v>7.6</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" ref="F13:F15" si="0">EXP(B$3+B13*C$3+C13*D$3+D13*E$3+E13*F$3)</f>
+        <v>1.0189474533055892E-2</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="28">
+        <v>10965</v>
+      </c>
+      <c r="C14" s="28">
+        <v>1.9</v>
+      </c>
+      <c r="D14" s="28">
+        <v>2</v>
+      </c>
+      <c r="E14" s="28">
+        <v>5</v>
+      </c>
+      <c r="F14" s="28">
+        <f t="shared" si="0"/>
+        <v>1.0066270483375141E-2</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="6">
+        <v>30000</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>-15.4</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0067931555039549E-2</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="6">
+        <v>15800</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>4.0487500000000001</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" ref="F16" si="1">EXP(B$3+B16*C$3+C16*D$3+D16*E$3+E16*F$3)</f>
+        <v>1.0024281291303708E-2</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E17" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" ref="F17" si="2">EXP(B$3+B17*C$3+C17*D$3+D17*E$3+E17*F$3)</f>
+        <v>1.0051333165410939E-2</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="6">
+        <v>500</v>
+      </c>
+      <c r="C18" s="6">
+        <v>2</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E18" s="6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" ref="F18" si="3">EXP(B$3+B18*C$3+C18*D$3+D18*E$3+E18*F$3)</f>
+        <v>1.0050328082349392E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="I11:K11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1019,12 +2474,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -1172,33 +2627,33 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="10"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1394,19 +2849,19 @@
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="22">
-        <v>0</v>
-      </c>
-      <c r="C20" s="22">
+      <c r="B20" s="21">
+        <v>0</v>
+      </c>
+      <c r="C20" s="21">
         <v>1.31</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="21">
         <v>100</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="23">
         <f>EXP(B$3+B20*C$3+C20*D$3+D20*E$3)</f>
         <v>3.3873592854351216E-2</v>
       </c>
@@ -1424,7 +2879,601 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="6"/>
+    <col min="6" max="6" width="12" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="27">
+        <v>0.962418</v>
+      </c>
+      <c r="C3" s="27">
+        <v>6.8640000000000003E-3</v>
+      </c>
+      <c r="D3" s="27">
+        <v>-0.30466199999999999</v>
+      </c>
+      <c r="E3" s="27">
+        <v>-0.14974399999999999</v>
+      </c>
+      <c r="F3" s="27">
+        <v>0.10487</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6">
+        <v>30000</v>
+      </c>
+      <c r="D6" s="6">
+        <v>100</v>
+      </c>
+      <c r="E6" s="6">
+        <v>54.46</v>
+      </c>
+      <c r="F6" s="6">
+        <v>91.69</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" ref="D7:F8" si="0">LOG(D5+1)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>2.0043213737826426</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>1.7439798652418428</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9670328821587024</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="26"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="26"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="str">
+        <f>C2</f>
+        <v>biomass</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>D2</f>
+        <v>loglc200</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>E2</f>
+        <v>loglf1000</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f>F2</f>
+        <v>loglf500</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1.31</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" ref="F13" si="1">EXP(B$3+B13*C$3+C13*D$3+D13*E$3+E13*F$3)</f>
+        <v>1.3018974535886614</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="28">
+        <v>10000</v>
+      </c>
+      <c r="C14" s="28">
+        <v>2</v>
+      </c>
+      <c r="D14" s="28">
+        <v>2</v>
+      </c>
+      <c r="E14" s="28">
+        <v>2</v>
+      </c>
+      <c r="F14" s="28">
+        <f t="shared" ref="F14:F19" si="2">EXP(B$3+B14*C$3+C14*D$3+D14*E$3+E14*F$3)</f>
+        <v>8.4012315077822805E+29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="28">
+        <v>30000</v>
+      </c>
+      <c r="C15" s="28">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28">
+        <v>0</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0</v>
+      </c>
+      <c r="F15" s="28">
+        <f t="shared" si="2"/>
+        <v>7.0451872457616263E+89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="28">
+        <v>0</v>
+      </c>
+      <c r="C16" s="28">
+        <v>0</v>
+      </c>
+      <c r="D16" s="28">
+        <v>0</v>
+      </c>
+      <c r="E16" s="28">
+        <v>0</v>
+      </c>
+      <c r="F16" s="28">
+        <f t="shared" si="2"/>
+        <v>2.6180191965875594</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="21">
+        <v>0</v>
+      </c>
+      <c r="C17" s="21">
+        <v>2</v>
+      </c>
+      <c r="D17" s="21">
+        <v>2</v>
+      </c>
+      <c r="E17" s="21">
+        <v>2</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="2"/>
+        <v>1.3012768828703487</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="21">
+        <v>100</v>
+      </c>
+      <c r="C18" s="21">
+        <v>2</v>
+      </c>
+      <c r="D18" s="21">
+        <v>2</v>
+      </c>
+      <c r="E18" s="21">
+        <v>2</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="2"/>
+        <v>2.5850529724651405</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="21">
+        <v>200</v>
+      </c>
+      <c r="C19" s="21">
+        <v>2</v>
+      </c>
+      <c r="D19" s="21">
+        <v>2</v>
+      </c>
+      <c r="E19" s="21">
+        <v>2</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="2"/>
+        <v>5.1353397254784445</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="21">
+        <v>300</v>
+      </c>
+      <c r="C20" s="21">
+        <v>2</v>
+      </c>
+      <c r="D20" s="21">
+        <v>2</v>
+      </c>
+      <c r="E20" s="21">
+        <v>2</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" ref="F20:F21" si="3">EXP(B$3+B20*C$3+C20*D$3+D20*E$3+E20*F$3)</f>
+        <v>10.201614580814022</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="21">
+        <v>400</v>
+      </c>
+      <c r="C21" s="21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="21">
+        <v>2</v>
+      </c>
+      <c r="E21" s="21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" si="3"/>
+        <v>20.266028270560252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="21">
+        <v>500</v>
+      </c>
+      <c r="C22" s="21">
+        <v>2</v>
+      </c>
+      <c r="D22" s="21">
+        <v>2</v>
+      </c>
+      <c r="E22" s="21">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" ref="F22" si="4">EXP(B$3+B22*C$3+C22*D$3+D22*E$3+E22*F$3)</f>
+        <v>40.259499965384421</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="21">
+        <v>0</v>
+      </c>
+      <c r="C23" s="21">
+        <v>0</v>
+      </c>
+      <c r="D23" s="21">
+        <v>0</v>
+      </c>
+      <c r="E23" s="21">
+        <v>0</v>
+      </c>
+      <c r="F23" s="6">
+        <f>EXP(B$3+B23*C$3+C23*D$3+D23*E$3+E23*F$3)</f>
+        <v>2.6180191965875594</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="21">
+        <v>100</v>
+      </c>
+      <c r="C24" s="21">
+        <v>0</v>
+      </c>
+      <c r="D24" s="21">
+        <v>0</v>
+      </c>
+      <c r="E24" s="21">
+        <v>0</v>
+      </c>
+      <c r="F24" s="6">
+        <f>EXP(B$3+B24*C$3+C24*D$3+D24*E$3+E24*F$3)</f>
+        <v>5.2008288129896521</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="21">
+        <v>200</v>
+      </c>
+      <c r="C25" s="21">
+        <v>0</v>
+      </c>
+      <c r="D25" s="21">
+        <v>0</v>
+      </c>
+      <c r="E25" s="21">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6">
+        <f>EXP(B$3+B25*C$3+C25*D$3+D25*E$3+E25*F$3)</f>
+        <v>10.331711997100602</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="21">
+        <v>300</v>
+      </c>
+      <c r="C26" s="21">
+        <v>0</v>
+      </c>
+      <c r="D26" s="21">
+        <v>0</v>
+      </c>
+      <c r="E26" s="21">
+        <v>0</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" ref="F26:F27" si="5">EXP(B$3+B26*C$3+C26*D$3+D26*E$3+E26*F$3)</f>
+        <v>20.52447343093214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="21">
+        <v>400</v>
+      </c>
+      <c r="C27" s="21">
+        <v>0</v>
+      </c>
+      <c r="D27" s="21">
+        <v>0</v>
+      </c>
+      <c r="E27" s="21">
+        <v>0</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="5"/>
+        <v>40.772914472960167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="21">
+        <v>500</v>
+      </c>
+      <c r="C28" s="21">
+        <v>0</v>
+      </c>
+      <c r="D28" s="21">
+        <v>0</v>
+      </c>
+      <c r="E28" s="21">
+        <v>0</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" ref="F28" si="6">EXP(B$3+B28*C$3+C28*D$3+D28*E$3+E28*F$3)</f>
+        <v>80.997476510841892</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="I11:K11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -1441,10 +3490,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19"/>
+      <c r="C1" s="29"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -1569,16 +3618,16 @@
       <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1589,9 +3638,9 @@
       <c r="C11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
       <c r="G11" s="10"/>
       <c r="H11" s="12"/>
     </row>
@@ -1646,13 +3695,13 @@
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="22">
-        <v>0</v>
-      </c>
-      <c r="C15" s="24">
+      <c r="B15" s="21">
+        <v>0</v>
+      </c>
+      <c r="C15" s="23">
         <f>EXP(B$3+B15*C$3)</f>
         <v>5.0612084504354105E-3</v>
       </c>
@@ -1675,12 +3724,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,13 +3743,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
@@ -1742,11 +3791,11 @@
       <c r="D3" s="16">
         <v>0.2732</v>
       </c>
-      <c r="E3" s="23">
-        <f t="shared" ref="C3:F3" si="0">LN(E4)</f>
+      <c r="E3" s="22">
+        <f t="shared" ref="E3" si="0">LN(E4)</f>
         <v>2.0430000000000101E-2</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="24">
         <v>5.8819999999999998E-6</v>
       </c>
       <c r="G3" s="8"/>
@@ -1793,6 +3842,9 @@
       <c r="E5" s="6">
         <v>0.31</v>
       </c>
+      <c r="F5" s="6">
+        <v>0.09</v>
+      </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -1811,6 +3863,9 @@
       </c>
       <c r="E6" s="6">
         <v>99.28</v>
+      </c>
+      <c r="F6" s="6">
+        <v>30000</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -1862,34 +3917,34 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
       <c r="F11" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2114,27 +4169,24 @@
       <c r="L19" s="11"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="22">
-        <v>0</v>
-      </c>
-      <c r="C20" s="22">
-        <v>7.46</v>
-      </c>
-      <c r="D20" s="22">
+      <c r="B20" s="21">
+        <v>0</v>
+      </c>
+      <c r="C20" s="21">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="D20" s="21">
         <v>100</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="21">
         <v>10965</v>
       </c>
-      <c r="F20" s="24">
+      <c r="F20" s="23">
         <f>EXP(B$3+B20*C$3+C20*D$3+D20*E$3+E20*F$3)</f>
-        <v>13.021061084954049</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>32</v>
+        <v>17.442192546705737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>